<commit_message>
preparing data for ISSI poster
</commit_message>
<xml_diff>
--- a/data/data_cases.xlsx
+++ b/data/data_cases.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\R\tu-case-1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\R\tu-case-1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E9C0A1-4A21-4FB3-8B06-214478D47A39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C1591C-8715-4507-97DA-F60DEB3B9CF0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{B60B1D78-A8D8-4951-BCE0-7EB73145C67A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B60B1D78-A8D8-4951-BCE0-7EB73145C67A}"/>
   </bookViews>
   <sheets>
     <sheet name="bio_data" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="poster_examples" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bio_data!$A$1:$R$387</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3527" uniqueCount="1029">
   <si>
     <t>institution</t>
   </si>
@@ -3527,22 +3532,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7A9297-2EDB-42DD-9C55-FAFE6D99F2C2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H201" sqref="H201"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:R376"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>542</v>
       </c>
@@ -3598,7 +3604,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>557</v>
       </c>
@@ -3636,7 +3642,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>558</v>
       </c>
@@ -3665,7 +3671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>559</v>
       </c>
@@ -3694,7 +3700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>560</v>
       </c>
@@ -3723,7 +3729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>561</v>
       </c>
@@ -3752,7 +3758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>562</v>
       </c>
@@ -3781,7 +3787,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>563</v>
       </c>
@@ -3810,7 +3816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>564</v>
       </c>
@@ -3842,7 +3848,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>565</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>567</v>
       </c>
@@ -3900,7 +3906,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>566</v>
       </c>
@@ -3929,7 +3935,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>568</v>
       </c>
@@ -3958,7 +3964,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>569</v>
       </c>
@@ -3987,7 +3993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>570</v>
       </c>
@@ -4016,7 +4022,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>571</v>
       </c>
@@ -4045,7 +4051,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>572</v>
       </c>
@@ -4074,7 +4080,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>573</v>
       </c>
@@ -4109,7 +4115,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>574</v>
       </c>
@@ -4138,7 +4144,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>575</v>
       </c>
@@ -4170,7 +4176,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>576</v>
       </c>
@@ -4199,7 +4205,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>577</v>
       </c>
@@ -4231,7 +4237,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>578</v>
       </c>
@@ -4260,7 +4266,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>579</v>
       </c>
@@ -4289,7 +4295,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>580</v>
       </c>
@@ -4318,7 +4324,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>581</v>
       </c>
@@ -4347,7 +4353,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>582</v>
       </c>
@@ -4376,7 +4382,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>583</v>
       </c>
@@ -4405,7 +4411,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>584</v>
       </c>
@@ -4434,7 +4440,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>585</v>
       </c>
@@ -4463,7 +4469,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>586</v>
       </c>
@@ -4492,7 +4498,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>587</v>
       </c>
@@ -4521,7 +4527,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>588</v>
       </c>
@@ -4550,7 +4556,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>589</v>
       </c>
@@ -4579,7 +4585,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>590</v>
       </c>
@@ -4608,7 +4614,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>591</v>
       </c>
@@ -4640,7 +4646,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>592</v>
       </c>
@@ -4672,7 +4678,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>593</v>
       </c>
@@ -4701,7 +4707,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>594</v>
       </c>
@@ -4733,7 +4739,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>595</v>
       </c>
@@ -4762,7 +4768,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>596</v>
       </c>
@@ -4791,7 +4797,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>597</v>
       </c>
@@ -4820,7 +4826,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>598</v>
       </c>
@@ -4858,7 +4864,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>599</v>
       </c>
@@ -4887,7 +4893,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>600</v>
       </c>
@@ -4916,7 +4922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>601</v>
       </c>
@@ -4945,7 +4951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>602</v>
       </c>
@@ -4974,7 +4980,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>603</v>
       </c>
@@ -5003,7 +5009,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>604</v>
       </c>
@@ -5032,7 +5038,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>605</v>
       </c>
@@ -5061,7 +5067,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>606</v>
       </c>
@@ -5090,7 +5096,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>607</v>
       </c>
@@ -5122,7 +5128,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>608</v>
       </c>
@@ -5151,7 +5157,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>609</v>
       </c>
@@ -5180,7 +5186,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>610</v>
       </c>
@@ -5209,7 +5215,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>611</v>
       </c>
@@ -5235,7 +5241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>612</v>
       </c>
@@ -5264,7 +5270,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>613</v>
       </c>
@@ -5293,7 +5299,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>614</v>
       </c>
@@ -5325,7 +5331,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>615</v>
       </c>
@@ -5354,7 +5360,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>616</v>
       </c>
@@ -5383,7 +5389,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>617</v>
       </c>
@@ -5412,7 +5418,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>618</v>
       </c>
@@ -5441,7 +5447,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>619</v>
       </c>
@@ -5470,7 +5476,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>620</v>
       </c>
@@ -5499,7 +5505,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>621</v>
       </c>
@@ -5528,7 +5534,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>622</v>
       </c>
@@ -5557,7 +5563,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>623</v>
       </c>
@@ -5589,7 +5595,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>624</v>
       </c>
@@ -5618,7 +5624,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>625</v>
       </c>
@@ -5647,7 +5653,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>626</v>
       </c>
@@ -5676,7 +5682,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>627</v>
       </c>
@@ -5705,7 +5711,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>628</v>
       </c>
@@ -5734,7 +5740,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>629</v>
       </c>
@@ -5763,7 +5769,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>630</v>
       </c>
@@ -5792,7 +5798,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>631</v>
       </c>
@@ -5821,7 +5827,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>632</v>
       </c>
@@ -5850,7 +5856,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>633</v>
       </c>
@@ -5879,7 +5885,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>634</v>
       </c>
@@ -5908,7 +5914,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>635</v>
       </c>
@@ -5940,7 +5946,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>636</v>
       </c>
@@ -5969,7 +5975,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>637</v>
       </c>
@@ -5998,7 +6004,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>638</v>
       </c>
@@ -6027,7 +6033,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>639</v>
       </c>
@@ -6059,7 +6065,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>640</v>
       </c>
@@ -6088,7 +6094,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>641</v>
       </c>
@@ -6117,7 +6123,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>642</v>
       </c>
@@ -6146,7 +6152,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>643</v>
       </c>
@@ -6178,7 +6184,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>644</v>
       </c>
@@ -6207,7 +6213,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>645</v>
       </c>
@@ -6236,7 +6242,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>646</v>
       </c>
@@ -6265,7 +6271,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>647</v>
       </c>
@@ -6294,7 +6300,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>648</v>
       </c>
@@ -6323,7 +6329,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>649</v>
       </c>
@@ -6352,7 +6358,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>650</v>
       </c>
@@ -6384,7 +6390,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>651</v>
       </c>
@@ -6413,7 +6419,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>652</v>
       </c>
@@ -6442,7 +6448,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>653</v>
       </c>
@@ -6471,7 +6477,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>654</v>
       </c>
@@ -6500,7 +6506,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>655</v>
       </c>
@@ -6533,7 +6539,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>656</v>
       </c>
@@ -6562,7 +6568,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>657</v>
       </c>
@@ -6591,7 +6597,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>658</v>
       </c>
@@ -6620,7 +6626,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>659</v>
       </c>
@@ -6649,7 +6655,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>660</v>
       </c>
@@ -6678,7 +6684,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>661</v>
       </c>
@@ -6707,7 +6713,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>662</v>
       </c>
@@ -6736,7 +6742,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>663</v>
       </c>
@@ -6765,7 +6771,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>664</v>
       </c>
@@ -6797,7 +6803,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>543</v>
       </c>
@@ -6826,7 +6832,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>544</v>
       </c>
@@ -6855,7 +6861,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>545</v>
       </c>
@@ -6884,7 +6890,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>546</v>
       </c>
@@ -6916,7 +6922,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>547</v>
       </c>
@@ -6948,7 +6954,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>548</v>
       </c>
@@ -6980,7 +6986,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>549</v>
       </c>
@@ -7009,7 +7015,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>550</v>
       </c>
@@ -7038,7 +7044,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>551</v>
       </c>
@@ -7067,7 +7073,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>552</v>
       </c>
@@ -7096,7 +7102,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>553</v>
       </c>
@@ -7125,7 +7131,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>554</v>
       </c>
@@ -7154,7 +7160,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>555</v>
       </c>
@@ -7183,7 +7189,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>556</v>
       </c>
@@ -7212,7 +7218,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>665</v>
       </c>
@@ -7241,7 +7247,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>666</v>
       </c>
@@ -7270,7 +7276,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>667</v>
       </c>
@@ -7299,7 +7305,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>668</v>
       </c>
@@ -7328,7 +7334,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>669</v>
       </c>
@@ -7360,7 +7366,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>670</v>
       </c>
@@ -7389,7 +7395,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>671</v>
       </c>
@@ -7418,7 +7424,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>672</v>
       </c>
@@ -7447,7 +7453,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>673</v>
       </c>
@@ -7479,7 +7485,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>674</v>
       </c>
@@ -7508,7 +7514,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>675</v>
       </c>
@@ -7549,7 +7555,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>676</v>
       </c>
@@ -7587,7 +7593,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>677</v>
       </c>
@@ -7625,7 +7631,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>678</v>
       </c>
@@ -7663,7 +7669,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>679</v>
       </c>
@@ -7701,7 +7707,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>680</v>
       </c>
@@ -7739,7 +7745,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>681</v>
       </c>
@@ -7777,7 +7783,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>682</v>
       </c>
@@ -7818,7 +7824,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>683</v>
       </c>
@@ -7856,7 +7862,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>684</v>
       </c>
@@ -7891,7 +7897,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>685</v>
       </c>
@@ -7929,7 +7935,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>686</v>
       </c>
@@ -7967,7 +7973,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>687</v>
       </c>
@@ -8005,7 +8011,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>688</v>
       </c>
@@ -8043,7 +8049,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>689</v>
       </c>
@@ -8081,7 +8087,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>690</v>
       </c>
@@ -8119,7 +8125,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>691</v>
       </c>
@@ -8157,7 +8163,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>692</v>
       </c>
@@ -8198,7 +8204,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>693</v>
       </c>
@@ -8236,7 +8242,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>694</v>
       </c>
@@ -8274,7 +8280,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>695</v>
       </c>
@@ -8315,7 +8321,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>696</v>
       </c>
@@ -8353,7 +8359,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>697</v>
       </c>
@@ -8391,7 +8397,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>698</v>
       </c>
@@ -8432,7 +8438,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>699</v>
       </c>
@@ -8470,7 +8476,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>700</v>
       </c>
@@ -8508,7 +8514,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>701</v>
       </c>
@@ -8546,7 +8552,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>702</v>
       </c>
@@ -8584,7 +8590,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>703</v>
       </c>
@@ -8622,7 +8628,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>704</v>
       </c>
@@ -8660,7 +8666,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>705</v>
       </c>
@@ -8698,7 +8704,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>706</v>
       </c>
@@ -8736,7 +8742,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>707</v>
       </c>
@@ -8774,7 +8780,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>708</v>
       </c>
@@ -8812,7 +8818,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>709</v>
       </c>
@@ -8850,7 +8856,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>710</v>
       </c>
@@ -8888,7 +8894,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>711</v>
       </c>
@@ -8926,7 +8932,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>712</v>
       </c>
@@ -8964,7 +8970,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>713</v>
       </c>
@@ -9002,7 +9008,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>714</v>
       </c>
@@ -9043,7 +9049,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>715</v>
       </c>
@@ -9081,7 +9087,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>716</v>
       </c>
@@ -9119,7 +9125,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>717</v>
       </c>
@@ -9157,7 +9163,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>718</v>
       </c>
@@ -9195,7 +9201,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>719</v>
       </c>
@@ -9233,7 +9239,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>720</v>
       </c>
@@ -9271,7 +9277,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>721</v>
       </c>
@@ -9309,7 +9315,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>722</v>
       </c>
@@ -9347,7 +9353,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>723</v>
       </c>
@@ -9385,7 +9391,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>724</v>
       </c>
@@ -9423,7 +9429,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>725</v>
       </c>
@@ -9461,7 +9467,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>726</v>
       </c>
@@ -9499,7 +9505,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>727</v>
       </c>
@@ -9537,7 +9543,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>728</v>
       </c>
@@ -9575,7 +9581,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>729</v>
       </c>
@@ -9613,7 +9619,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>730</v>
       </c>
@@ -9648,7 +9654,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>731</v>
       </c>
@@ -9683,7 +9689,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>732</v>
       </c>
@@ -9712,7 +9718,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>733</v>
       </c>
@@ -9741,7 +9747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>734</v>
       </c>
@@ -9770,7 +9776,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>735</v>
       </c>
@@ -9799,7 +9805,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>736</v>
       </c>
@@ -9828,7 +9834,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>737</v>
       </c>
@@ -9854,7 +9860,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>738</v>
       </c>
@@ -9880,7 +9886,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>739</v>
       </c>
@@ -9906,7 +9912,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>740</v>
       </c>
@@ -9932,7 +9938,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>741</v>
       </c>
@@ -9967,7 +9973,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>742</v>
       </c>
@@ -9990,7 +9996,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>743</v>
       </c>
@@ -10013,7 +10019,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>744</v>
       </c>
@@ -10036,7 +10042,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>745</v>
       </c>
@@ -10059,7 +10065,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>746</v>
       </c>
@@ -10082,7 +10088,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>747</v>
       </c>
@@ -10105,7 +10111,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>748</v>
       </c>
@@ -10128,7 +10134,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>749</v>
       </c>
@@ -10151,7 +10157,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>750</v>
       </c>
@@ -10174,7 +10180,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>751</v>
       </c>
@@ -10197,7 +10203,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>752</v>
       </c>
@@ -10220,7 +10226,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>753</v>
       </c>
@@ -10243,7 +10249,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>754</v>
       </c>
@@ -10266,7 +10272,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>755</v>
       </c>
@@ -10289,7 +10295,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>756</v>
       </c>
@@ -10312,7 +10318,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>757</v>
       </c>
@@ -10341,7 +10347,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>758</v>
       </c>
@@ -10370,7 +10376,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>759</v>
       </c>
@@ -10399,7 +10405,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>760</v>
       </c>
@@ -10431,7 +10437,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>761</v>
       </c>
@@ -10460,7 +10466,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>762</v>
       </c>
@@ -10489,7 +10495,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>763</v>
       </c>
@@ -10521,7 +10527,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>764</v>
       </c>
@@ -10550,7 +10556,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>765</v>
       </c>
@@ -10579,7 +10585,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>766</v>
       </c>
@@ -10608,7 +10614,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>767</v>
       </c>
@@ -10637,7 +10643,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>768</v>
       </c>
@@ -10669,7 +10675,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>769</v>
       </c>
@@ -10698,7 +10704,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>770</v>
       </c>
@@ -10730,7 +10736,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>771</v>
       </c>
@@ -10759,7 +10765,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>772</v>
       </c>
@@ -10791,7 +10797,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>773</v>
       </c>
@@ -10820,7 +10826,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>774</v>
       </c>
@@ -10849,7 +10855,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>775</v>
       </c>
@@ -10881,7 +10887,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>776</v>
       </c>
@@ -10910,7 +10916,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>777</v>
       </c>
@@ -10939,7 +10945,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>778</v>
       </c>
@@ -10968,7 +10974,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>779</v>
       </c>
@@ -10997,7 +11003,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>780</v>
       </c>
@@ -11023,7 +11029,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>781</v>
       </c>
@@ -11049,7 +11055,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>782</v>
       </c>
@@ -11075,7 +11081,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>783</v>
       </c>
@@ -11101,7 +11107,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>784</v>
       </c>
@@ -11127,7 +11133,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>785</v>
       </c>
@@ -11153,7 +11159,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>786</v>
       </c>
@@ -11179,7 +11185,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>787</v>
       </c>
@@ -11205,7 +11211,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>788</v>
       </c>
@@ -11231,7 +11237,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>789</v>
       </c>
@@ -11257,7 +11263,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>790</v>
       </c>
@@ -11283,7 +11289,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>791</v>
       </c>
@@ -11309,7 +11315,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>792</v>
       </c>
@@ -11335,7 +11341,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>793</v>
       </c>
@@ -11361,7 +11367,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>794</v>
       </c>
@@ -11387,7 +11393,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>795</v>
       </c>
@@ -11413,7 +11419,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>796</v>
       </c>
@@ -11439,7 +11445,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>797</v>
       </c>
@@ -11465,7 +11471,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>798</v>
       </c>
@@ -11491,7 +11497,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>799</v>
       </c>
@@ -11517,7 +11523,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>800</v>
       </c>
@@ -11543,7 +11549,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>801</v>
       </c>
@@ -11569,7 +11575,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>802</v>
       </c>
@@ -11595,7 +11601,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>803</v>
       </c>
@@ -11621,7 +11627,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>804</v>
       </c>
@@ -11647,7 +11653,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>805</v>
       </c>
@@ -11673,7 +11679,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>806</v>
       </c>
@@ -11699,7 +11705,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>807</v>
       </c>
@@ -11725,7 +11731,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>808</v>
       </c>
@@ -11751,7 +11757,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>809</v>
       </c>
@@ -11777,7 +11783,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>810</v>
       </c>
@@ -11803,7 +11809,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>811</v>
       </c>
@@ -11829,7 +11835,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>812</v>
       </c>
@@ -11855,7 +11861,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>813</v>
       </c>
@@ -11881,7 +11887,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>814</v>
       </c>
@@ -11907,7 +11913,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>815</v>
       </c>
@@ -11933,7 +11939,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>816</v>
       </c>
@@ -11959,7 +11965,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>817</v>
       </c>
@@ -11985,7 +11991,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>818</v>
       </c>
@@ -12011,7 +12017,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>819</v>
       </c>
@@ -12037,7 +12043,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>820</v>
       </c>
@@ -12063,7 +12069,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>821</v>
       </c>
@@ -12089,7 +12095,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>822</v>
       </c>
@@ -12115,7 +12121,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>823</v>
       </c>
@@ -12141,7 +12147,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>824</v>
       </c>
@@ -12167,7 +12173,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>825</v>
       </c>
@@ -12193,7 +12199,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>826</v>
       </c>
@@ -12219,7 +12225,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>827</v>
       </c>
@@ -12245,7 +12251,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>828</v>
       </c>
@@ -12271,7 +12277,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>829</v>
       </c>
@@ -12297,7 +12303,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>830</v>
       </c>
@@ -12323,7 +12329,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>831</v>
       </c>
@@ -12349,7 +12355,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>832</v>
       </c>
@@ -12375,7 +12381,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>833</v>
       </c>
@@ -12401,7 +12407,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>834</v>
       </c>
@@ -12427,7 +12433,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>835</v>
       </c>
@@ -12453,7 +12459,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>836</v>
       </c>
@@ -12479,7 +12485,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>837</v>
       </c>
@@ -12505,7 +12511,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>838</v>
       </c>
@@ -12531,7 +12537,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>839</v>
       </c>
@@ -12557,7 +12563,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>840</v>
       </c>
@@ -12583,7 +12589,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>841</v>
       </c>
@@ -12609,7 +12615,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>842</v>
       </c>
@@ -12635,7 +12641,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>843</v>
       </c>
@@ -12661,7 +12667,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>844</v>
       </c>
@@ -12687,7 +12693,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>845</v>
       </c>
@@ -12713,7 +12719,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>846</v>
       </c>
@@ -12739,7 +12745,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>847</v>
       </c>
@@ -12765,7 +12771,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>848</v>
       </c>
@@ -12791,7 +12797,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>849</v>
       </c>
@@ -12817,7 +12823,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>850</v>
       </c>
@@ -12843,7 +12849,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>851</v>
       </c>
@@ -12869,7 +12875,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>852</v>
       </c>
@@ -12895,7 +12901,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>853</v>
       </c>
@@ -12921,7 +12927,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>854</v>
       </c>
@@ -12947,7 +12953,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>855</v>
       </c>
@@ -12973,7 +12979,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>856</v>
       </c>
@@ -12999,7 +13005,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>857</v>
       </c>
@@ -13025,7 +13031,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>858</v>
       </c>
@@ -13051,7 +13057,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>859</v>
       </c>
@@ -13077,7 +13083,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>860</v>
       </c>
@@ -13103,7 +13109,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>861</v>
       </c>
@@ -13129,7 +13135,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>862</v>
       </c>
@@ -13155,7 +13161,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>863</v>
       </c>
@@ -13181,7 +13187,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>864</v>
       </c>
@@ -13207,7 +13213,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>865</v>
       </c>
@@ -13233,7 +13239,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>866</v>
       </c>
@@ -13259,7 +13265,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>867</v>
       </c>
@@ -13285,7 +13291,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>868</v>
       </c>
@@ -13311,7 +13317,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>869</v>
       </c>
@@ -13337,7 +13343,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>870</v>
       </c>
@@ -13363,7 +13369,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>871</v>
       </c>
@@ -13389,7 +13395,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>872</v>
       </c>
@@ -13415,7 +13421,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>873</v>
       </c>
@@ -13441,7 +13447,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>874</v>
       </c>
@@ -13467,7 +13473,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>875</v>
       </c>
@@ -13493,7 +13499,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>876</v>
       </c>
@@ -13519,7 +13525,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>877</v>
       </c>
@@ -13545,7 +13551,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>878</v>
       </c>
@@ -13571,7 +13577,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>879</v>
       </c>
@@ -13597,7 +13603,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>880</v>
       </c>
@@ -13623,7 +13629,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>881</v>
       </c>
@@ -13649,7 +13655,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>882</v>
       </c>
@@ -13675,7 +13681,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>883</v>
       </c>
@@ -13701,7 +13707,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>884</v>
       </c>
@@ -13727,7 +13733,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>885</v>
       </c>
@@ -13753,7 +13759,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>886</v>
       </c>
@@ -13779,7 +13785,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>887</v>
       </c>
@@ -13805,7 +13811,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>888</v>
       </c>
@@ -13831,7 +13837,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>889</v>
       </c>
@@ -13857,7 +13863,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>890</v>
       </c>
@@ -13883,7 +13889,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>891</v>
       </c>
@@ -13909,7 +13915,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>892</v>
       </c>
@@ -13935,7 +13941,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>893</v>
       </c>
@@ -13961,7 +13967,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>894</v>
       </c>
@@ -13987,7 +13993,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>895</v>
       </c>
@@ -14016,7 +14022,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>896</v>
       </c>
@@ -14045,7 +14051,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>897</v>
       </c>
@@ -14074,7 +14080,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>898</v>
       </c>
@@ -14103,7 +14109,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>899</v>
       </c>
@@ -14132,7 +14138,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>900</v>
       </c>
@@ -14161,7 +14167,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>901</v>
       </c>
@@ -14190,7 +14196,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>902</v>
       </c>
@@ -14216,7 +14222,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>903</v>
       </c>
@@ -14242,7 +14248,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>904</v>
       </c>
@@ -14268,7 +14274,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>905</v>
       </c>
@@ -14294,7 +14300,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>906</v>
       </c>
@@ -14320,7 +14326,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>907</v>
       </c>
@@ -14346,7 +14352,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>908</v>
       </c>
@@ -14372,7 +14378,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>909</v>
       </c>
@@ -14398,7 +14404,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>910</v>
       </c>
@@ -14424,7 +14430,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>911</v>
       </c>
@@ -14450,7 +14456,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>912</v>
       </c>
@@ -14476,7 +14482,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>913</v>
       </c>
@@ -14502,7 +14508,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>914</v>
       </c>
@@ -14528,7 +14534,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>915</v>
       </c>
@@ -14554,7 +14560,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>916</v>
       </c>
@@ -14580,7 +14586,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>917</v>
       </c>
@@ -14606,7 +14612,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>918</v>
       </c>
@@ -14632,7 +14638,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>919</v>
       </c>
@@ -14658,7 +14664,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>920</v>
       </c>
@@ -14684,7 +14690,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>921</v>
       </c>
@@ -14710,7 +14716,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>922</v>
       </c>
@@ -14736,7 +14742,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>923</v>
       </c>
@@ -14762,7 +14768,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>924</v>
       </c>
@@ -14788,7 +14794,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>925</v>
       </c>
@@ -14814,7 +14820,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>926</v>
       </c>
@@ -14840,7 +14846,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>927</v>
       </c>
@@ -14866,7 +14872,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>928</v>
       </c>
@@ -14893,6 +14899,89 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R387" xr:uid="{2FCFB6BC-4CA9-4F5B-A3FE-2070F35BC9B2}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Social Sciences and Humanities"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="10603581"/>
+        <filter val="11437613"/>
+        <filter val="11959747"/>
+        <filter val="12587609;12587611;12587606"/>
+        <filter val="13692131"/>
+        <filter val="13712719;13712718"/>
+        <filter val="13742361"/>
+        <filter val="13948010;13948009"/>
+        <filter val="14500378"/>
+        <filter val="16624485"/>
+        <filter val="16983346"/>
+        <filter val="17343667"/>
+        <filter val="17444478"/>
+        <filter val="17554352"/>
+        <filter val="18234320"/>
+        <filter val="18371611"/>
+        <filter val="19041624;19041864"/>
+        <filter val="19043192;19043194"/>
+        <filter val="19133580"/>
+        <filter val="19325628"/>
+        <filter val="19866764"/>
+        <filter val="20130196"/>
+        <filter val="22626126"/>
+        <filter val="23921773"/>
+        <filter val="24635618;24635973"/>
+        <filter val="24681715"/>
+        <filter val="25100281"/>
+        <filter val="2854669"/>
+        <filter val="29003178"/>
+        <filter val="2901"/>
+        <filter val="29141698;29141697"/>
+        <filter val="29344056"/>
+        <filter val="29371432"/>
+        <filter val="30434714"/>
+        <filter val="32966855"/>
+        <filter val="33209862"/>
+        <filter val="333740"/>
+        <filter val="33449014"/>
+        <filter val="33898806"/>
+        <filter val="33916285"/>
+        <filter val="34506521"/>
+        <filter val="34586176"/>
+        <filter val="35411041"/>
+        <filter val="35538177"/>
+        <filter val="36789409"/>
+        <filter val="36871407"/>
+        <filter val="3838893"/>
+        <filter val="39757127"/>
+        <filter val="40046625;40046628"/>
+        <filter val="40851367"/>
+        <filter val="40973442;40973443"/>
+        <filter val="41017620"/>
+        <filter val="41201274"/>
+        <filter val="414336"/>
+        <filter val="45577199"/>
+        <filter val="45717564;45717623;45717662"/>
+        <filter val="47342790"/>
+        <filter val="47434469;47434467;47434470;47434468"/>
+        <filter val="47748745"/>
+        <filter val="50356306"/>
+        <filter val="50373155"/>
+        <filter val="51114439"/>
+        <filter val="51330433;51330438"/>
+        <filter val="5521084"/>
+        <filter val="6318608"/>
+        <filter val="7113418;7113420"/>
+        <filter val="7443016"/>
+        <filter val="8106965"/>
+        <filter val="8216129;8216131"/>
+        <filter val="8458971"/>
+        <filter val="8634446;8636593;8637313"/>
+        <filter val="9724845"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="N134" r:id="rId1" xr:uid="{5376E815-CA1F-4D3D-9FE3-8C7487C3688B}"/>
     <hyperlink ref="N135" r:id="rId2" xr:uid="{1789C6AA-13A2-4181-B460-7EEE5CAF2397}"/>
@@ -14919,9 +15008,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>536</v>
       </c>
@@ -14932,7 +15021,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>505</v>
       </c>
@@ -14943,11 +15032,1104 @@
         <v>538</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6369285-517D-4CF3-BBE7-78D5A0310167}">
+  <dimension ref="A1:C98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>775</v>
+      </c>
+      <c r="B2">
+        <v>13692131</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>777</v>
+      </c>
+      <c r="B3">
+        <v>24635618</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>777</v>
+      </c>
+      <c r="B4">
+        <v>24635973</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>778</v>
+      </c>
+      <c r="B5">
+        <v>6318608</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>779</v>
+      </c>
+      <c r="B6">
+        <v>16624485</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>780</v>
+      </c>
+      <c r="B7">
+        <v>7443016</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>781</v>
+      </c>
+      <c r="B8">
+        <v>13692131</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>782</v>
+      </c>
+      <c r="B9">
+        <v>24635618</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>782</v>
+      </c>
+      <c r="B10">
+        <v>24635973</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>783</v>
+      </c>
+      <c r="B11">
+        <v>6318608</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>784</v>
+      </c>
+      <c r="B12">
+        <v>3838893</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>785</v>
+      </c>
+      <c r="B13">
+        <v>8634446</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>785</v>
+      </c>
+      <c r="B14">
+        <v>8636593</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>785</v>
+      </c>
+      <c r="B15">
+        <v>8637313</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>786</v>
+      </c>
+      <c r="B16">
+        <v>13712719</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>786</v>
+      </c>
+      <c r="B17">
+        <v>13712718</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>788</v>
+      </c>
+      <c r="B18">
+        <v>13948010</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>788</v>
+      </c>
+      <c r="B19">
+        <v>13948009</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>789</v>
+      </c>
+      <c r="B20">
+        <v>40046625</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>789</v>
+      </c>
+      <c r="B21">
+        <v>40046628</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>790</v>
+      </c>
+      <c r="B22">
+        <v>19043192</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>790</v>
+      </c>
+      <c r="B23">
+        <v>19043194</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>791</v>
+      </c>
+      <c r="B24">
+        <v>23921773</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>792</v>
+      </c>
+      <c r="B25">
+        <v>11437613</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>793</v>
+      </c>
+      <c r="B26">
+        <v>33449014</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>794</v>
+      </c>
+      <c r="B27">
+        <v>33916285</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>795</v>
+      </c>
+      <c r="B28">
+        <v>24681715</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>797</v>
+      </c>
+      <c r="B29">
+        <v>29003178</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>798</v>
+      </c>
+      <c r="B30">
+        <v>45717564</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>798</v>
+      </c>
+      <c r="B31">
+        <v>45717623</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>798</v>
+      </c>
+      <c r="B32">
+        <v>45717662</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>799</v>
+      </c>
+      <c r="B33">
+        <v>41201274</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>800</v>
+      </c>
+      <c r="B34">
+        <v>2901</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>801</v>
+      </c>
+      <c r="B35">
+        <v>19866764</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>802</v>
+      </c>
+      <c r="B36">
+        <v>8216129</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>802</v>
+      </c>
+      <c r="B37">
+        <v>8216131</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>804</v>
+      </c>
+      <c r="B38">
+        <v>50373155</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>805</v>
+      </c>
+      <c r="B39">
+        <v>14500378</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>806</v>
+      </c>
+      <c r="B40">
+        <v>18234320</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>807</v>
+      </c>
+      <c r="B41">
+        <v>36789409</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>808</v>
+      </c>
+      <c r="B42">
+        <v>32966855</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>809</v>
+      </c>
+      <c r="B43">
+        <v>12587609</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>809</v>
+      </c>
+      <c r="B44">
+        <v>12587611</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>809</v>
+      </c>
+      <c r="B45">
+        <v>12587606</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>810</v>
+      </c>
+      <c r="B46">
+        <v>5521084</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>811</v>
+      </c>
+      <c r="B47">
+        <v>20130196</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>812</v>
+      </c>
+      <c r="B48">
+        <v>8458971</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>813</v>
+      </c>
+      <c r="B49">
+        <v>16624485</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>814</v>
+      </c>
+      <c r="B50">
+        <v>41017620</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>815</v>
+      </c>
+      <c r="B51">
+        <v>19325628</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>816</v>
+      </c>
+      <c r="B52">
+        <v>51330433</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>816</v>
+      </c>
+      <c r="B53">
+        <v>51330438</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>817</v>
+      </c>
+      <c r="B54">
+        <v>19041624</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>817</v>
+      </c>
+      <c r="B55">
+        <v>19041864</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>818</v>
+      </c>
+      <c r="B56">
+        <v>414336</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>819</v>
+      </c>
+      <c r="B57">
+        <v>2854669</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>821</v>
+      </c>
+      <c r="B58">
+        <v>16983346</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>822</v>
+      </c>
+      <c r="B59">
+        <v>47434469</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>822</v>
+      </c>
+      <c r="B60">
+        <v>47434467</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>822</v>
+      </c>
+      <c r="B61">
+        <v>47434470</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>822</v>
+      </c>
+      <c r="B62">
+        <v>47434468</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>823</v>
+      </c>
+      <c r="B63">
+        <v>40851367</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>824</v>
+      </c>
+      <c r="B64">
+        <v>34506521</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>825</v>
+      </c>
+      <c r="B65">
+        <v>30434714</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>826</v>
+      </c>
+      <c r="B66">
+        <v>34586176</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>827</v>
+      </c>
+      <c r="B67">
+        <v>35411041</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>828</v>
+      </c>
+      <c r="B68">
+        <v>22626126</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>829</v>
+      </c>
+      <c r="B69">
+        <v>13742361</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>830</v>
+      </c>
+      <c r="B70">
+        <v>40973442</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>830</v>
+      </c>
+      <c r="B71">
+        <v>40973443</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>831</v>
+      </c>
+      <c r="B72">
+        <v>39757127</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>832</v>
+      </c>
+      <c r="B73">
+        <v>51114439</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>837</v>
+      </c>
+      <c r="B74" s="1">
+        <v>17444478</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>838</v>
+      </c>
+      <c r="B75">
+        <v>33898806</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>841</v>
+      </c>
+      <c r="B76">
+        <v>17554352</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>847</v>
+      </c>
+      <c r="B77">
+        <v>29344056</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>852</v>
+      </c>
+      <c r="B78">
+        <v>47748745</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>857</v>
+      </c>
+      <c r="B79">
+        <v>29371432</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>859</v>
+      </c>
+      <c r="B80">
+        <v>45577199</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>865</v>
+      </c>
+      <c r="B81">
+        <v>11959747</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>874</v>
+      </c>
+      <c r="B82">
+        <v>47342790</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>879</v>
+      </c>
+      <c r="B83">
+        <v>17343667</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>881</v>
+      </c>
+      <c r="B84">
+        <v>10603581</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>894</v>
+      </c>
+      <c r="B85">
+        <v>19133580</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>901</v>
+      </c>
+      <c r="B86">
+        <v>36871407</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>902</v>
+      </c>
+      <c r="B87">
+        <v>333740</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>903</v>
+      </c>
+      <c r="B88">
+        <v>9724845</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>904</v>
+      </c>
+      <c r="B89">
+        <v>8106965</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>906</v>
+      </c>
+      <c r="B90">
+        <v>7113418</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>906</v>
+      </c>
+      <c r="B91">
+        <v>7113420</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>907</v>
+      </c>
+      <c r="B92">
+        <v>35538177</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>908</v>
+      </c>
+      <c r="B93">
+        <v>29141698</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>908</v>
+      </c>
+      <c r="B94">
+        <v>29141697</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>910</v>
+      </c>
+      <c r="B95">
+        <v>33209862</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>915</v>
+      </c>
+      <c r="B96">
+        <v>50356306</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>916</v>
+      </c>
+      <c r="B97">
+        <v>25100281</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>917</v>
+      </c>
+      <c r="B98">
+        <v>18371611</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
included data for examples for poster
</commit_message>
<xml_diff>
--- a/data/data_cases.xlsx
+++ b/data/data_cases.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\R\tu-case-1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C1591C-8715-4507-97DA-F60DEB3B9CF0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AE1F35-958F-4B6C-82E0-C74E68899DCF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B60B1D78-A8D8-4951-BCE0-7EB73145C67A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{B60B1D78-A8D8-4951-BCE0-7EB73145C67A}"/>
   </bookViews>
   <sheets>
     <sheet name="bio_data" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
     <sheet name="poster_examples" sheetId="3" r:id="rId3"/>
+    <sheet name="poster_data" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bio_data!$A$1:$R$387</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">poster_data!$A$1:$N$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3527" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="1042">
   <si>
     <t>institution</t>
   </si>
@@ -3123,6 +3125,45 @@
   </si>
   <si>
     <t>https://pure.tudelft.nl/portal/en/persons/sjp-callens(83741046-08ed-41f4-8255-cef348cef6cf)/publications.html</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>first_year</t>
+  </si>
+  <si>
+    <t>last_year</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>oa_p</t>
+  </si>
+  <si>
+    <t>news_m</t>
+  </si>
+  <si>
+    <t>pol_m</t>
+  </si>
+  <si>
+    <t>p_w_young</t>
+  </si>
+  <si>
+    <t>co_aut</t>
+  </si>
+  <si>
+    <t>fund_p</t>
+  </si>
+  <si>
+    <t>pp_oa</t>
+  </si>
+  <si>
+    <t>pp_w_young</t>
+  </si>
+  <si>
+    <t>pp_fund</t>
   </si>
 </sst>
 </file>
@@ -15045,8 +15086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6369285-517D-4CF3-BBE7-78D5A0310167}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16132,4 +16173,3632 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9CF9108-9A5A-4C07-B425-6634E1D8C76A}">
+  <dimension ref="A1:N82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>901</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>2000</v>
+      </c>
+      <c r="D2">
+        <v>2018</v>
+      </c>
+      <c r="E2">
+        <v>77</v>
+      </c>
+      <c r="F2">
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <v>65</v>
+      </c>
+      <c r="H2">
+        <v>57</v>
+      </c>
+      <c r="I2">
+        <v>41</v>
+      </c>
+      <c r="J2">
+        <v>90</v>
+      </c>
+      <c r="K2">
+        <v>19</v>
+      </c>
+      <c r="L2">
+        <v>0.27272727272727298</v>
+      </c>
+      <c r="M2">
+        <v>0.27272727272727298</v>
+      </c>
+      <c r="N2">
+        <v>0.246753246753247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>777</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
+      <c r="D3">
+        <v>2017</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>27</v>
+      </c>
+      <c r="J3">
+        <v>65</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M3">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="N3">
+        <v>6.6666666666666693E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>782</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>2017</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>27</v>
+      </c>
+      <c r="J4">
+        <v>65</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M4">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="N4">
+        <v>6.6666666666666693E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>780</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>1992</v>
+      </c>
+      <c r="D5">
+        <v>2017</v>
+      </c>
+      <c r="E5">
+        <v>84</v>
+      </c>
+      <c r="F5">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5">
+        <v>80</v>
+      </c>
+      <c r="I5">
+        <v>67</v>
+      </c>
+      <c r="J5">
+        <v>105</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>0.226190476190476</v>
+      </c>
+      <c r="M5">
+        <v>0.226190476190476</v>
+      </c>
+      <c r="N5">
+        <v>7.1428571428571397E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>775</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>2005</v>
+      </c>
+      <c r="D6">
+        <v>2018</v>
+      </c>
+      <c r="E6">
+        <v>52</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>49</v>
+      </c>
+      <c r="K6">
+        <v>16</v>
+      </c>
+      <c r="L6">
+        <v>0.32692307692307698</v>
+      </c>
+      <c r="M6">
+        <v>0.32692307692307698</v>
+      </c>
+      <c r="N6">
+        <v>0.30769230769230799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>781</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2005</v>
+      </c>
+      <c r="D7">
+        <v>2018</v>
+      </c>
+      <c r="E7">
+        <v>52</v>
+      </c>
+      <c r="F7">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>49</v>
+      </c>
+      <c r="K7">
+        <v>16</v>
+      </c>
+      <c r="L7">
+        <v>0.32692307692307698</v>
+      </c>
+      <c r="M7">
+        <v>0.32692307692307698</v>
+      </c>
+      <c r="N7">
+        <v>0.30769230769230799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>799</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>2009</v>
+      </c>
+      <c r="D8">
+        <v>2018</v>
+      </c>
+      <c r="E8">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>18</v>
+      </c>
+      <c r="J8">
+        <v>32</v>
+      </c>
+      <c r="K8">
+        <v>11</v>
+      </c>
+      <c r="L8">
+        <v>0.77272727272727304</v>
+      </c>
+      <c r="M8">
+        <v>0.77272727272727304</v>
+      </c>
+      <c r="N8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>792</v>
+      </c>
+      <c r="B9">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>1991</v>
+      </c>
+      <c r="D9">
+        <v>2017</v>
+      </c>
+      <c r="E9">
+        <v>31</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>22</v>
+      </c>
+      <c r="J9">
+        <v>55</v>
+      </c>
+      <c r="K9">
+        <v>17</v>
+      </c>
+      <c r="L9">
+        <v>0.45161290322580599</v>
+      </c>
+      <c r="M9">
+        <v>0.45161290322580599</v>
+      </c>
+      <c r="N9">
+        <v>0.54838709677419395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>794</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>1997</v>
+      </c>
+      <c r="D10">
+        <v>2017</v>
+      </c>
+      <c r="E10">
+        <v>54</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>46</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <v>0.240740740740741</v>
+      </c>
+      <c r="M10">
+        <v>0.240740740740741</v>
+      </c>
+      <c r="N10">
+        <v>0.11111111111111099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>809</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>2008</v>
+      </c>
+      <c r="D11">
+        <v>2018</v>
+      </c>
+      <c r="E11">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>31</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="M11">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="N11">
+        <v>0.17857142857142899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>816</v>
+      </c>
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>1998</v>
+      </c>
+      <c r="D12">
+        <v>2017</v>
+      </c>
+      <c r="E12">
+        <v>37</v>
+      </c>
+      <c r="F12">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>29</v>
+      </c>
+      <c r="J12">
+        <v>59</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <v>0.32432432432432401</v>
+      </c>
+      <c r="M12">
+        <v>0.32432432432432401</v>
+      </c>
+      <c r="N12">
+        <v>0.21621621621621601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>816</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>2017</v>
+      </c>
+      <c r="D13">
+        <v>2017</v>
+      </c>
+      <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>29</v>
+      </c>
+      <c r="J13">
+        <v>59</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>0.32432432432432401</v>
+      </c>
+      <c r="M13">
+        <v>0.32432432432432401</v>
+      </c>
+      <c r="N13">
+        <v>0.21621621621621601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>798</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>2009</v>
+      </c>
+      <c r="D14">
+        <v>2018</v>
+      </c>
+      <c r="E14">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14">
+        <v>17</v>
+      </c>
+      <c r="J14">
+        <v>41</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>0.40909090909090901</v>
+      </c>
+      <c r="M14">
+        <v>0.40909090909090901</v>
+      </c>
+      <c r="N14">
+        <v>0.54545454545454497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>798</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>2010</v>
+      </c>
+      <c r="D15">
+        <v>2017</v>
+      </c>
+      <c r="E15">
+        <v>22</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>17</v>
+      </c>
+      <c r="J15">
+        <v>41</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>0.40909090909090901</v>
+      </c>
+      <c r="M15">
+        <v>0.40909090909090901</v>
+      </c>
+      <c r="N15">
+        <v>0.54545454545454497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>778</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>2008</v>
+      </c>
+      <c r="D16">
+        <v>2017</v>
+      </c>
+      <c r="E16">
+        <v>17</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>28</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>0.47058823529411797</v>
+      </c>
+      <c r="M16">
+        <v>0.47058823529411797</v>
+      </c>
+      <c r="N16">
+        <v>5.8823529411764698E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>783</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>2008</v>
+      </c>
+      <c r="D17">
+        <v>2017</v>
+      </c>
+      <c r="E17">
+        <v>17</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>28</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0.47058823529411797</v>
+      </c>
+      <c r="M17">
+        <v>0.47058823529411797</v>
+      </c>
+      <c r="N17">
+        <v>5.8823529411764698E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>789</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>2002</v>
+      </c>
+      <c r="D18">
+        <v>2017</v>
+      </c>
+      <c r="E18">
+        <v>49</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>34</v>
+      </c>
+      <c r="J18">
+        <v>55</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>0.16326530612244899</v>
+      </c>
+      <c r="M18">
+        <v>0.16326530612244899</v>
+      </c>
+      <c r="N18">
+        <v>8.1632653061224497E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>791</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>2002</v>
+      </c>
+      <c r="D19">
+        <v>2017</v>
+      </c>
+      <c r="E19">
+        <v>27</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>43</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0.296296296296296</v>
+      </c>
+      <c r="M19">
+        <v>0.296296296296296</v>
+      </c>
+      <c r="N19">
+        <v>3.7037037037037E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>795</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>2009</v>
+      </c>
+      <c r="D20">
+        <v>2018</v>
+      </c>
+      <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>22</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="M20">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="N20">
+        <v>0.230769230769231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>785</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>2000</v>
+      </c>
+      <c r="D21">
+        <v>2018</v>
+      </c>
+      <c r="E21">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>11</v>
+      </c>
+      <c r="J21">
+        <v>32</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>797</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>2009</v>
+      </c>
+      <c r="D22">
+        <v>2017</v>
+      </c>
+      <c r="E22">
+        <v>23</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>14</v>
+      </c>
+      <c r="J22">
+        <v>29</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>0.30434782608695699</v>
+      </c>
+      <c r="M22">
+        <v>0.30434782608695699</v>
+      </c>
+      <c r="N22">
+        <v>4.3478260869565202E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>786</v>
+      </c>
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <v>2003</v>
+      </c>
+      <c r="D23">
+        <v>2018</v>
+      </c>
+      <c r="E23">
+        <v>40</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>47</v>
+      </c>
+      <c r="J23">
+        <v>80</v>
+      </c>
+      <c r="K23">
+        <v>7</v>
+      </c>
+      <c r="L23">
+        <v>0.15</v>
+      </c>
+      <c r="M23">
+        <v>0.15</v>
+      </c>
+      <c r="N23">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>788</v>
+      </c>
+      <c r="B24">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>1982</v>
+      </c>
+      <c r="D24">
+        <v>2017</v>
+      </c>
+      <c r="E24">
+        <v>28</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>13</v>
+      </c>
+      <c r="J24">
+        <v>28</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="M24">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>788</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>2013</v>
+      </c>
+      <c r="D25">
+        <v>2013</v>
+      </c>
+      <c r="E25">
+        <v>28</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>13</v>
+      </c>
+      <c r="J25">
+        <v>28</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="M25">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>815</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>2012</v>
+      </c>
+      <c r="D26">
+        <v>2017</v>
+      </c>
+      <c r="E26">
+        <v>9</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>11</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="M26">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="N26">
+        <v>0.11111111111111099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>903</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>2010</v>
+      </c>
+      <c r="D27">
+        <v>2018</v>
+      </c>
+      <c r="E27">
+        <v>24</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>15</v>
+      </c>
+      <c r="I27">
+        <v>6</v>
+      </c>
+      <c r="J27">
+        <v>14</v>
+      </c>
+      <c r="K27">
+        <v>12</v>
+      </c>
+      <c r="L27">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="M27">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="N27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>904</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>2011</v>
+      </c>
+      <c r="D28">
+        <v>2017</v>
+      </c>
+      <c r="E28">
+        <v>17</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>14</v>
+      </c>
+      <c r="K28">
+        <v>11</v>
+      </c>
+      <c r="L28">
+        <v>0.29411764705882398</v>
+      </c>
+      <c r="M28">
+        <v>0.29411764705882398</v>
+      </c>
+      <c r="N28">
+        <v>0.64705882352941202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>790</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>2011</v>
+      </c>
+      <c r="D29">
+        <v>2017</v>
+      </c>
+      <c r="E29">
+        <v>11</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>14</v>
+      </c>
+      <c r="J29">
+        <v>29</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="M29">
+        <v>0.45454545454545497</v>
+      </c>
+      <c r="N29">
+        <v>0.27272727272727298</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>804</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>2013</v>
+      </c>
+      <c r="D30">
+        <v>2018</v>
+      </c>
+      <c r="E30">
+        <v>9</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>18</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="M30">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="N30">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>817</v>
+      </c>
+      <c r="B31">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>2001</v>
+      </c>
+      <c r="D31">
+        <v>2018</v>
+      </c>
+      <c r="E31">
+        <v>20</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>18</v>
+      </c>
+      <c r="J31">
+        <v>38</v>
+      </c>
+      <c r="K31">
+        <v>6</v>
+      </c>
+      <c r="L31">
+        <v>0.25</v>
+      </c>
+      <c r="M31">
+        <v>0.25</v>
+      </c>
+      <c r="N31">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>805</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>2009</v>
+      </c>
+      <c r="D32">
+        <v>2018</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>14</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="M32">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="N32">
+        <v>0.66666666666666696</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>822</v>
+      </c>
+      <c r="B33">
+        <v>23</v>
+      </c>
+      <c r="C33">
+        <v>1994</v>
+      </c>
+      <c r="D33">
+        <v>2017</v>
+      </c>
+      <c r="E33">
+        <v>11</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>25</v>
+      </c>
+      <c r="J33">
+        <v>33</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="M33">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="N33">
+        <v>0.18181818181818199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>822</v>
+      </c>
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>2005</v>
+      </c>
+      <c r="D34">
+        <v>2017</v>
+      </c>
+      <c r="E34">
+        <v>11</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>25</v>
+      </c>
+      <c r="J34">
+        <v>33</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+      <c r="L34">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="M34">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="N34">
+        <v>0.18181818181818199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>907</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>2014</v>
+      </c>
+      <c r="D35">
+        <v>2017</v>
+      </c>
+      <c r="E35">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>7</v>
+      </c>
+      <c r="K35">
+        <v>8</v>
+      </c>
+      <c r="L35">
+        <v>0.25</v>
+      </c>
+      <c r="M35">
+        <v>0.25</v>
+      </c>
+      <c r="N35">
+        <v>0.66666666666666696</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>908</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>2005</v>
+      </c>
+      <c r="D36">
+        <v>2016</v>
+      </c>
+      <c r="E36">
+        <v>21</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="J36">
+        <v>26</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="M36">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="N36">
+        <v>9.5238095238095205E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>908</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>2015</v>
+      </c>
+      <c r="D37">
+        <v>2015</v>
+      </c>
+      <c r="E37">
+        <v>21</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="I37">
+        <v>8</v>
+      </c>
+      <c r="J37">
+        <v>26</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="M37">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="N37">
+        <v>9.5238095238095205E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>793</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>2000</v>
+      </c>
+      <c r="D38">
+        <v>2015</v>
+      </c>
+      <c r="E38">
+        <v>23</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>7</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38">
+        <v>24</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0.13043478260869601</v>
+      </c>
+      <c r="M38">
+        <v>0.13043478260869601</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>800</v>
+      </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>2012</v>
+      </c>
+      <c r="D39">
+        <v>2018</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>7</v>
+      </c>
+      <c r="K39">
+        <v>2</v>
+      </c>
+      <c r="L39">
+        <v>0.3</v>
+      </c>
+      <c r="M39">
+        <v>0.3</v>
+      </c>
+      <c r="N39">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>810</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>2016</v>
+      </c>
+      <c r="D40">
+        <v>2017</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>6</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>0.6</v>
+      </c>
+      <c r="M40">
+        <v>0.6</v>
+      </c>
+      <c r="N40">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>824</v>
+      </c>
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>1997</v>
+      </c>
+      <c r="D41">
+        <v>2007</v>
+      </c>
+      <c r="E41">
+        <v>9</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="J41">
+        <v>14</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M41">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>852</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>2016</v>
+      </c>
+      <c r="D42">
+        <v>2017</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+      <c r="K42">
+        <v>3</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>881</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>2016</v>
+      </c>
+      <c r="D43">
+        <v>2017</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>8</v>
+      </c>
+      <c r="K43">
+        <v>4</v>
+      </c>
+      <c r="L43">
+        <v>0.75</v>
+      </c>
+      <c r="M43">
+        <v>0.75</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>808</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>2014</v>
+      </c>
+      <c r="D44">
+        <v>2017</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <v>11</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <v>0.5</v>
+      </c>
+      <c r="M44">
+        <v>0.5</v>
+      </c>
+      <c r="N44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>811</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>2011</v>
+      </c>
+      <c r="D45">
+        <v>2017</v>
+      </c>
+      <c r="E45">
+        <v>9</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>8</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="M45">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="N45">
+        <v>0.11111111111111099</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>814</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>2009</v>
+      </c>
+      <c r="D46">
+        <v>2018</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>5</v>
+      </c>
+      <c r="J46">
+        <v>17</v>
+      </c>
+      <c r="K46">
+        <v>2</v>
+      </c>
+      <c r="L46">
+        <v>0.25</v>
+      </c>
+      <c r="M46">
+        <v>0.25</v>
+      </c>
+      <c r="N46">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>825</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>2012</v>
+      </c>
+      <c r="D47">
+        <v>2018</v>
+      </c>
+      <c r="E47">
+        <v>24</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>9</v>
+      </c>
+      <c r="I47">
+        <v>8</v>
+      </c>
+      <c r="J47">
+        <v>33</v>
+      </c>
+      <c r="K47">
+        <v>13</v>
+      </c>
+      <c r="L47">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="M47">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="N47">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>831</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>2014</v>
+      </c>
+      <c r="D48">
+        <v>2017</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>4</v>
+      </c>
+      <c r="J48">
+        <v>8</v>
+      </c>
+      <c r="K48">
+        <v>2</v>
+      </c>
+      <c r="L48">
+        <v>0.5</v>
+      </c>
+      <c r="M48">
+        <v>0.5</v>
+      </c>
+      <c r="N48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>837</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>2012</v>
+      </c>
+      <c r="D49">
+        <v>2016</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>902</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>2012</v>
+      </c>
+      <c r="D50">
+        <v>2016</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>18</v>
+      </c>
+      <c r="J50">
+        <v>33</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0.125</v>
+      </c>
+      <c r="M50">
+        <v>0.125</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>906</v>
+      </c>
+      <c r="B51">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>2004</v>
+      </c>
+      <c r="D51">
+        <v>2018</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <v>5</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M51">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>915</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>2016</v>
+      </c>
+      <c r="D52">
+        <v>2016</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <v>27</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>784</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>2007</v>
+      </c>
+      <c r="D53">
+        <v>2007</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>5</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>802</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>2008</v>
+      </c>
+      <c r="D54">
+        <v>2015</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>6</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M54">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="N54">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>806</v>
+      </c>
+      <c r="B55">
+        <v>11</v>
+      </c>
+      <c r="C55">
+        <v>2006</v>
+      </c>
+      <c r="D55">
+        <v>2017</v>
+      </c>
+      <c r="E55">
+        <v>7</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>11</v>
+      </c>
+      <c r="K55">
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="M55">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="N55">
+        <v>0.42857142857142899</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>807</v>
+      </c>
+      <c r="B56">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>2004</v>
+      </c>
+      <c r="D56">
+        <v>2017</v>
+      </c>
+      <c r="E56">
+        <v>9</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>8</v>
+      </c>
+      <c r="I56">
+        <v>9</v>
+      </c>
+      <c r="J56">
+        <v>17</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="M56">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>812</v>
+      </c>
+      <c r="B57">
+        <v>12</v>
+      </c>
+      <c r="C57">
+        <v>2006</v>
+      </c>
+      <c r="D57">
+        <v>2018</v>
+      </c>
+      <c r="E57">
+        <v>13</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>6</v>
+      </c>
+      <c r="I57">
+        <v>9</v>
+      </c>
+      <c r="J57">
+        <v>29</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>7.69230769230769E-2</v>
+      </c>
+      <c r="M57">
+        <v>7.69230769230769E-2</v>
+      </c>
+      <c r="N57">
+        <v>7.69230769230769E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>819</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>2017</v>
+      </c>
+      <c r="D58">
+        <v>2017</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>4</v>
+      </c>
+      <c r="J58">
+        <v>8</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>823</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>2018</v>
+      </c>
+      <c r="D59">
+        <v>2018</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>4</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>830</v>
+      </c>
+      <c r="B60">
+        <v>32</v>
+      </c>
+      <c r="C60">
+        <v>1985</v>
+      </c>
+      <c r="D60">
+        <v>2017</v>
+      </c>
+      <c r="E60">
+        <v>10</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>9</v>
+      </c>
+      <c r="J60">
+        <v>14</v>
+      </c>
+      <c r="K60">
+        <v>4</v>
+      </c>
+      <c r="L60">
+        <v>0.1</v>
+      </c>
+      <c r="M60">
+        <v>0.1</v>
+      </c>
+      <c r="N60">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>838</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <v>2012</v>
+      </c>
+      <c r="D61">
+        <v>2016</v>
+      </c>
+      <c r="E61">
+        <v>4</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>3</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0.25</v>
+      </c>
+      <c r="M61">
+        <v>0.25</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>859</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <v>2013</v>
+      </c>
+      <c r="D62">
+        <v>2016</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+      <c r="K62">
+        <v>3</v>
+      </c>
+      <c r="L62">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M62">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>865</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>2017</v>
+      </c>
+      <c r="D63">
+        <v>2017</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>879</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>2017</v>
+      </c>
+      <c r="D64">
+        <v>2017</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>4</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>894</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>2017</v>
+      </c>
+      <c r="D65">
+        <v>2017</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>2</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <v>1</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>910</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>2017</v>
+      </c>
+      <c r="D66">
+        <v>2017</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>3</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>916</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>2013</v>
+      </c>
+      <c r="D67">
+        <v>2013</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>3</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>917</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>2016</v>
+      </c>
+      <c r="D68">
+        <v>2016</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>8</v>
+      </c>
+      <c r="J68">
+        <v>8</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>779</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>2017</v>
+      </c>
+      <c r="D69">
+        <v>2017</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>2</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>801</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>2013</v>
+      </c>
+      <c r="D70">
+        <v>2018</v>
+      </c>
+      <c r="E70">
+        <v>5</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>8</v>
+      </c>
+      <c r="J70">
+        <v>14</v>
+      </c>
+      <c r="K70">
+        <v>2</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>813</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>2017</v>
+      </c>
+      <c r="D71">
+        <v>2017</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>2</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>818</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>2013</v>
+      </c>
+      <c r="D72">
+        <v>2013</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>2</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>821</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="C73">
+        <v>2014</v>
+      </c>
+      <c r="D73">
+        <v>2017</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>3</v>
+      </c>
+      <c r="K73">
+        <v>2</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0.66666666666666696</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>826</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+      <c r="C74">
+        <v>2010</v>
+      </c>
+      <c r="D74">
+        <v>2017</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74">
+        <v>5</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>827</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>2013</v>
+      </c>
+      <c r="D75">
+        <v>2013</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>2</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>828</v>
+      </c>
+      <c r="B76">
+        <v>6</v>
+      </c>
+      <c r="C76">
+        <v>2009</v>
+      </c>
+      <c r="D76">
+        <v>2015</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>2</v>
+      </c>
+      <c r="J76">
+        <v>5</v>
+      </c>
+      <c r="K76">
+        <v>2</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>829</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77">
+        <v>2015</v>
+      </c>
+      <c r="D77">
+        <v>2017</v>
+      </c>
+      <c r="E77">
+        <v>5</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>3</v>
+      </c>
+      <c r="K77">
+        <v>3</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>832</v>
+      </c>
+      <c r="B78">
+        <v>21</v>
+      </c>
+      <c r="C78">
+        <v>1994</v>
+      </c>
+      <c r="D78">
+        <v>2015</v>
+      </c>
+      <c r="E78">
+        <v>20</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>14</v>
+      </c>
+      <c r="I78">
+        <v>13</v>
+      </c>
+      <c r="J78">
+        <v>20</v>
+      </c>
+      <c r="K78">
+        <v>4</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>841</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>2017</v>
+      </c>
+      <c r="D79">
+        <v>2017</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>2</v>
+      </c>
+      <c r="J79">
+        <v>3</v>
+      </c>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>847</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>2014</v>
+      </c>
+      <c r="D80">
+        <v>2014</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>2</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>857</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>2015</v>
+      </c>
+      <c r="D81">
+        <v>2015</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>4</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>874</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>2016</v>
+      </c>
+      <c r="D82">
+        <v>2017</v>
+      </c>
+      <c r="E82">
+        <v>3</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>5</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N82" xr:uid="{196043E1-9538-40EE-9DCE-346E5046AE40}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N82">
+      <sortCondition descending="1" ref="F1:F82"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>